<commit_message>
Added sample list from Nov_2020 and notes
</commit_message>
<xml_diff>
--- a/metadata/E5_2020_Timeseries_Sample_Metadata_Sheet.xlsx
+++ b/metadata/E5_2020_Timeseries_Sample_Metadata_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcone\Documents\URI\Lab-Notebook\urol-e5\timeseries\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7779EB71-C17A-4672-84E1-A9A05954BDB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71102F65-4B55-4BF6-B4A5-BCE978D4C55B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11112" yWindow="2040" windowWidth="17280" windowHeight="9408" xr2:uid="{A9225978-0C17-4C60-8E40-23766E55B839}"/>
+    <workbookView xWindow="0" yWindow="2952" windowWidth="17280" windowHeight="9408" xr2:uid="{A9225978-0C17-4C60-8E40-23766E55B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="229">
   <si>
     <t>Coral_Species</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Dead as of Sept_2020</t>
   </si>
   <si>
-    <t>Mostly dead as of Mar_2020 ; ~98% dead as of Sept_2020</t>
-  </si>
-  <si>
     <t>Not found Sept_2020</t>
   </si>
   <si>
@@ -311,36 +308,15 @@
     <t>100% Dead as of Sept_2020</t>
   </si>
   <si>
-    <t>98% Dead as of Sept_2020</t>
-  </si>
-  <si>
-    <t>95% Dead as of Sept_2020</t>
-  </si>
-  <si>
-    <t>Not found Mar_2020; 95% Dead as of Sept_2020</t>
-  </si>
-  <si>
     <t>Alive but not sampled Sept_2020</t>
   </si>
   <si>
-    <t>Alive as of Sept_2020; HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED</t>
-  </si>
-  <si>
-    <t>Not found Mar_2020; 80% Dead in Sept_2020 ; HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED</t>
-  </si>
-  <si>
-    <t>Mostly dead as of Mar_2020 ; Fully Dead as of Sept_2020</t>
-  </si>
-  <si>
     <t>Alive, HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED</t>
   </si>
   <si>
     <t>50% Dead as of Sept_2020 - Not sampled</t>
   </si>
   <si>
-    <t>90% Dead as of Sept_2020 - Not sampled</t>
-  </si>
-  <si>
     <t>POC-40</t>
   </si>
   <si>
@@ -530,15 +506,9 @@
     <t>POC-395</t>
   </si>
   <si>
-    <t>No tag found Mar_2020 nor Sept_2020, now POC-230</t>
-  </si>
-  <si>
     <t>Photographed in Mar_2020 but no sample</t>
   </si>
   <si>
-    <t>No tag in Sept_2020 ; Retagged as POC-300</t>
-  </si>
-  <si>
     <t>POR-209</t>
   </si>
   <si>
@@ -632,52 +602,124 @@
     <t>Porites</t>
   </si>
   <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_38</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_98</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_62</t>
-  </si>
-  <si>
-    <t>Not found in Sept_2020</t>
-  </si>
-  <si>
-    <t>No tag in Mar_2020 ; Retagged as POR_206</t>
-  </si>
-  <si>
-    <t>No tag as of Sept_2020 ; Retagged as POR_271</t>
-  </si>
-  <si>
-    <t>No tag as of Sept_2020 ; Retagged as 204</t>
-  </si>
-  <si>
-    <t>Not found</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_298</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_299</t>
-  </si>
-  <si>
-    <t>Jan_2020 called POR_344 (tag is 341)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan_2020, Mar_2020 and Sept_2020 called POR_387 (tag is 385) ; Very confused the entire time </t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_399</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_397</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_39</t>
-  </si>
-  <si>
-    <t>No tag in Sept_2020 ; Retagged as POR_398</t>
+    <t>Only molecular taken Nov_2020</t>
+  </si>
+  <si>
+    <t>Mostly dead as of Mar_2020 ; ~98% dead as of Sept_2020 ; 100% dead as of Nov_2020</t>
+  </si>
+  <si>
+    <t>Not sure if correct coral sampled (three ACR colonies missing tags in Nov_2020) - now ACR_275 if correct coral</t>
+  </si>
+  <si>
+    <t>Not sure if correct coral sampled (three ACR colonies missing tags in Nov_2020) - now ACR_276 if correct coral</t>
+  </si>
+  <si>
+    <t>Not found Sept_2020 ; not found Nov_2020 either</t>
+  </si>
+  <si>
+    <t>New Tag as of Sept_2020 - Four colonies found in Sept_2020 and could not match from previous photos ; Mostly dead from spawning but still got phys and molec in Nov_2020</t>
+  </si>
+  <si>
+    <t>Not found Mar_2020 or Sept_2020, 100% Dead as of Nov_2020</t>
+  </si>
+  <si>
+    <t>100% Dead as of Sept_2020 and Nov_2020</t>
+  </si>
+  <si>
+    <t>98% Dead as of Sept_2020 and Nov_2020</t>
+  </si>
+  <si>
+    <t>95% Dead as of Sept_2020 and Nov_2020</t>
+  </si>
+  <si>
+    <t>99% Dead as of Sept_2020 ; 95% Dead as of Nov_2020</t>
+  </si>
+  <si>
+    <t>Not found Mar_2020; 95% Dead as of Sept_2020; 90% Dead as of Nov_2020</t>
+  </si>
+  <si>
+    <t>Alive as of Sept_2020; HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED ; NOV_2020 this colony was found but too dead to sample, also not photographed for some reason</t>
+  </si>
+  <si>
+    <t>Not found Mar_2020; 80% Dead in Sept_2020 ; HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED ; NOV_2020 this colony was found but too dead to sample, also not photographed for some reason</t>
+  </si>
+  <si>
+    <t>Mostly dead as of Mar_2020 ; Fully Dead as of Sept_2020; 98% Dead as of Nov_2020</t>
+  </si>
+  <si>
+    <t>Alive, HILTON NOT USED FOR SPAWNING SINCE MOST COLONIES DIED; NOV_2020 - Only molecular samples taken</t>
+  </si>
+  <si>
+    <t>Not found in Sept_2020 nor Nov_2020</t>
+  </si>
+  <si>
+    <t>Not found Sept_2020, nor Nov_2020</t>
+  </si>
+  <si>
+    <t>Not found in Nov_2020</t>
+  </si>
+  <si>
+    <t>Not found in Sept_2020, nor Nov_2020</t>
+  </si>
+  <si>
+    <t>No tag found Mar_2020 - retagged as 230. Evidence of sampling in Mar_2020 but did not make it back to watertable or sampling. Did not find in Sept_2020, nor Nov_2020</t>
+  </si>
+  <si>
+    <t>Re tagged as POC-261 as of NOV_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POC-300 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_38 in Sept_2020</t>
+  </si>
+  <si>
+    <t>Re tagged as POR-274 as of NOV_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_98 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_62 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag as of Sept_2020 ; Retagged as POR_271 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag as of Sept_2020 ; Retagged as POR_204 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_298 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_299 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Mar_2020 ; Retagged as POR_206 in Sept_2020 ; Nov_2020 3 molecular bags because initial samples were small</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_397 in Sept_2020</t>
+  </si>
+  <si>
+    <t>Jan_2020 called POR_344 (tag is actually 341)</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_399 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_39 in Sept_2020 ; Think I (DC) know which one we tagged in Sept_2020 but no evidence of tag and wasn't confident to sample</t>
+  </si>
+  <si>
+    <t>No tag in Sept_2020 ; Retagged as POR_398 in Sept_2020</t>
+  </si>
+  <si>
+    <t>No tag in Nov_2020 ; Retagged as POR_270 in Nov_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan_2020, Mar_2020, Sept_2020, and Nov_2020 called POR_387 (tag is 385 - verified from Jan and Mar field photos) ; Very confused the entire time ; No tag as of Nov_2020, now tagged as POR-296 </t>
+  </si>
+  <si>
+    <t>90% Dead as of Sept_2020 - Not sampled ; Nov_2020 called ACR_398 but tag is 396 from field photos</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2420B75-8665-4DB7-A7B4-8B4461FB7AD9}">
   <dimension ref="A1:O146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L136" sqref="L136"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,19 +1122,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1106,10 +1149,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>30</v>
@@ -1126,7 +1169,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1">
         <v>-17.476872</v>
@@ -1170,7 +1213,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1">
         <v>-17.476872</v>
@@ -1198,6 +1241,9 @@
       </c>
       <c r="M3" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1240,6 +1286,12 @@
       <c r="M4" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -1281,6 +1333,9 @@
       <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1320,13 +1375,16 @@
         <v>28</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>165</v>
       </c>
@@ -1366,11 +1424,14 @@
       <c r="M7" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>173</v>
       </c>
@@ -1408,7 +1469,13 @@
         <v>28</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1422,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1">
         <v>-17.476872</v>
@@ -1451,8 +1518,11 @@
       <c r="M9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>176</v>
       </c>
@@ -1490,7 +1560,13 @@
         <v>32</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1533,6 +1609,12 @@
       <c r="M11" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1572,7 +1654,10 @@
         <v>32</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1615,6 +1700,9 @@
       <c r="M13" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1656,6 +1744,9 @@
       <c r="M14" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1697,8 +1788,14 @@
       <c r="M15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>193</v>
       </c>
@@ -1738,8 +1835,11 @@
       <c r="M16" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N16" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O16" s="3" t="s">
-        <v>35</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1780,7 +1880,10 @@
         <v>28</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>31</v>
@@ -1794,7 +1897,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
@@ -1812,7 +1915,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>28</v>
@@ -1825,6 +1928,9 @@
       </c>
       <c r="M18" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1835,7 +1941,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1">
         <v>7</v>
@@ -1853,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>28</v>
@@ -1866,6 +1972,12 @@
       </c>
       <c r="M19" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1876,7 +1988,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1">
         <v>10</v>
@@ -1894,7 +2006,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>28</v>
@@ -1906,7 +2018,10 @@
         <v>28</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -1917,7 +2032,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1">
         <v>10</v>
@@ -1935,7 +2050,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>28</v>
@@ -1949,8 +2064,11 @@
       <c r="M21" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O21" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1961,7 +2079,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1">
         <v>6</v>
@@ -1979,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>28</v>
@@ -1991,7 +2109,10 @@
         <v>32</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2002,7 +2123,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1">
         <v>15</v>
@@ -2020,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>28</v>
@@ -2033,6 +2154,9 @@
       </c>
       <c r="M23" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2043,7 +2167,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2061,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>28</v>
@@ -2075,8 +2199,11 @@
       <c r="M24" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N24" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O24" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2087,7 +2214,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="1">
         <v>8</v>
@@ -2105,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>28</v>
@@ -2118,6 +2245,9 @@
       </c>
       <c r="M25" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -2128,10 +2258,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="1">
         <v>-17.487100000000002</v>
@@ -2146,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>28</v>
@@ -2160,8 +2290,11 @@
       <c r="M26" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N26" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -2172,7 +2305,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1">
         <v>14</v>
@@ -2190,7 +2323,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>28</v>
@@ -2204,8 +2337,11 @@
       <c r="M27" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2216,7 +2352,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1">
         <v>8</v>
@@ -2234,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>28</v>
@@ -2246,7 +2382,10 @@
         <v>32</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -2257,7 +2396,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="1">
         <v>9</v>
@@ -2275,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>28</v>
@@ -2289,8 +2428,11 @@
       <c r="M29" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -2301,7 +2443,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -2319,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>28</v>
@@ -2332,6 +2474,12 @@
       </c>
       <c r="M30" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -2342,7 +2490,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -2360,7 +2508,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>28</v>
@@ -2373,6 +2521,9 @@
       </c>
       <c r="M31" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -2383,7 +2534,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1">
         <v>16</v>
@@ -2401,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>29</v>
@@ -2415,8 +2566,11 @@
       <c r="M32" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N32" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -2427,7 +2581,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1">
         <v>7</v>
@@ -2445,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>29</v>
@@ -2459,8 +2613,11 @@
       <c r="M33" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N33" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -2471,10 +2628,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="1">
         <v>-17.487100000000002</v>
@@ -2483,13 +2640,13 @@
         <v>-149.88766000000001</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H34" s="1">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>29</v>
@@ -2503,8 +2660,11 @@
       <c r="M34" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N34" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -2515,10 +2675,10 @@
         <v>8</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="1">
         <v>-17.487100000000002</v>
@@ -2527,13 +2687,13 @@
         <v>-149.88766000000001</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H35" s="1">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>29</v>
@@ -2547,8 +2707,11 @@
       <c r="M35" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N35" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -2559,10 +2722,10 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="1">
         <v>-17.487100000000002</v>
@@ -2571,13 +2734,13 @@
         <v>-149.88766000000001</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H36" s="1">
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>29</v>
@@ -2591,11 +2754,14 @@
       <c r="M36" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N36" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O36" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>241</v>
       </c>
@@ -2603,10 +2769,10 @@
         <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E37" s="1">
         <v>-17.487100000000002</v>
@@ -2615,13 +2781,13 @@
         <v>-149.88766000000001</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H37" s="1">
         <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>29</v>
@@ -2633,10 +2799,13 @@
         <v>28</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2647,7 +2816,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1">
         <v>8</v>
@@ -2665,7 +2834,7 @@
         <v>3</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>28</v>
@@ -2679,8 +2848,11 @@
       <c r="M38" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N38" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>345</v>
       </c>
@@ -2688,10 +2860,10 @@
         <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" s="1">
         <v>-17.4815</v>
@@ -2706,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>28</v>
@@ -2720,11 +2892,14 @@
       <c r="M39" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N39" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O39" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>347</v>
       </c>
@@ -2732,7 +2907,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1">
         <v>14</v>
@@ -2750,7 +2925,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>32</v>
@@ -2764,11 +2939,14 @@
       <c r="M40" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N40" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O40" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>350</v>
       </c>
@@ -2776,7 +2954,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1">
         <v>4</v>
@@ -2794,7 +2972,7 @@
         <v>3</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>28</v>
@@ -2808,11 +2986,14 @@
       <c r="M41" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N41" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O41" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>351</v>
       </c>
@@ -2820,7 +3001,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1">
         <v>6</v>
@@ -2838,7 +3019,7 @@
         <v>3</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>28</v>
@@ -2852,11 +3033,14 @@
       <c r="M42" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N42" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O42" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>360</v>
       </c>
@@ -2864,7 +3048,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -2882,7 +3066,7 @@
         <v>3</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>29</v>
@@ -2896,8 +3080,11 @@
       <c r="M43" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N43" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O43" s="3" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -2908,7 +3095,7 @@
         <v>8</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D44" s="1">
         <v>7</v>
@@ -2926,7 +3113,7 @@
         <v>3</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>28</v>
@@ -2940,8 +3127,11 @@
       <c r="M44" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N44" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O44" s="3" t="s">
-        <v>94</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -2952,10 +3142,10 @@
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="1">
         <v>-17.4815</v>
@@ -2970,7 +3160,7 @@
         <v>3</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>28</v>
@@ -2983,6 +3173,12 @@
       </c>
       <c r="M45" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -2993,7 +3189,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="1">
         <v>15</v>
@@ -3011,7 +3207,7 @@
         <v>3</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>28</v>
@@ -3025,11 +3221,14 @@
       <c r="M46" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N46" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O46" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>370</v>
       </c>
@@ -3037,7 +3236,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -3055,7 +3254,7 @@
         <v>3</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>29</v>
@@ -3069,11 +3268,14 @@
       <c r="M47" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N47" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O47" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>374</v>
       </c>
@@ -3081,7 +3283,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D48" s="1">
         <v>8</v>
@@ -3099,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>28</v>
@@ -3113,11 +3315,14 @@
       <c r="M48" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N48" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O48" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>376</v>
       </c>
@@ -3125,10 +3330,10 @@
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E49" s="1">
         <v>-17.4815</v>
@@ -3143,7 +3348,7 @@
         <v>3</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>29</v>
@@ -3157,11 +3362,14 @@
       <c r="M49" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N49" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O49" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>379</v>
       </c>
@@ -3169,7 +3377,7 @@
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D50" s="1">
         <v>7</v>
@@ -3187,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>28</v>
@@ -3201,8 +3409,11 @@
       <c r="M50" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N50" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O50" s="3" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -3213,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D51" s="1">
         <v>6</v>
@@ -3231,7 +3442,7 @@
         <v>3</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>28</v>
@@ -3245,8 +3456,11 @@
       <c r="M51" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N51" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O51" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -3257,7 +3471,7 @@
         <v>8</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D52" s="1">
         <v>4</v>
@@ -3275,7 +3489,7 @@
         <v>3</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>28</v>
@@ -3289,8 +3503,11 @@
       <c r="M52" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N52" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O52" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -3301,7 +3518,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D53" s="1">
         <v>9</v>
@@ -3319,7 +3536,7 @@
         <v>3</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>28</v>
@@ -3333,11 +3550,14 @@
       <c r="M53" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N53" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O53" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>396</v>
       </c>
@@ -3345,10 +3565,10 @@
         <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E54" s="1">
         <v>-17.4815</v>
@@ -3363,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>28</v>
@@ -3377,8 +3597,11 @@
       <c r="M54" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N54" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O54" s="3" t="s">
-        <v>101</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3389,10 +3612,10 @@
         <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" s="1">
         <v>-17.4815</v>
@@ -3401,13 +3624,13 @@
         <v>-149.84907999999999</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H55" s="1">
         <v>3</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>28</v>
@@ -3421,8 +3644,11 @@
       <c r="M55" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N55" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O55" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -3430,10 +3656,10 @@
         <v>40</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>29</v>
@@ -3465,16 +3691,19 @@
       <c r="M56" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N56" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>41</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>29</v>
@@ -3506,8 +3735,11 @@
       <c r="M57" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N57" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O57" s="3" t="s">
-        <v>35</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -3515,10 +3747,10 @@
         <v>42</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>29</v>
@@ -3549,6 +3781,9 @@
       </c>
       <c r="M58" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -3556,10 +3791,10 @@
         <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>29</v>
@@ -3590,6 +3825,9 @@
       </c>
       <c r="M59" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -3597,10 +3835,10 @@
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>29</v>
@@ -3631,6 +3869,9 @@
       </c>
       <c r="M60" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -3638,10 +3879,10 @@
         <v>45</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>29</v>
@@ -3672,6 +3913,9 @@
       </c>
       <c r="M61" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -3679,10 +3923,10 @@
         <v>47</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>29</v>
@@ -3713,6 +3957,9 @@
       </c>
       <c r="M62" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -3720,10 +3967,10 @@
         <v>48</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>29</v>
@@ -3754,6 +4001,9 @@
       </c>
       <c r="M63" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -3761,10 +4011,10 @@
         <v>50</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>29</v>
@@ -3795,6 +4045,9 @@
       </c>
       <c r="M64" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
@@ -3802,10 +4055,10 @@
         <v>52</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>29</v>
@@ -3836,6 +4089,9 @@
       </c>
       <c r="M65" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
@@ -3843,10 +4099,10 @@
         <v>53</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>29</v>
@@ -3877,6 +4133,9 @@
       </c>
       <c r="M66" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -3884,10 +4143,10 @@
         <v>55</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>29</v>
@@ -3919,8 +4178,11 @@
       <c r="M67" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N67" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O67" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
@@ -3928,10 +4190,10 @@
         <v>56</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>29</v>
@@ -3963,8 +4225,11 @@
       <c r="M68" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N68" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O68" s="3" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -3972,10 +4237,10 @@
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>29</v>
@@ -4006,6 +4271,9 @@
       </c>
       <c r="M69" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
@@ -4013,10 +4281,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>29</v>
@@ -4047,6 +4315,9 @@
       </c>
       <c r="M70" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -4054,10 +4325,10 @@
         <v>200</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>29</v>
@@ -4075,7 +4346,7 @@
         <v>2</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>28</v>
@@ -4088,6 +4359,9 @@
       </c>
       <c r="M71" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -4095,10 +4369,10 @@
         <v>201</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>29</v>
@@ -4116,7 +4390,7 @@
         <v>2</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>28</v>
@@ -4129,6 +4403,12 @@
       </c>
       <c r="M72" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O72" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
@@ -4136,10 +4416,10 @@
         <v>205</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>29</v>
@@ -4157,7 +4437,7 @@
         <v>2</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>28</v>
@@ -4170,6 +4450,9 @@
       </c>
       <c r="M73" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
@@ -4177,10 +4460,10 @@
         <v>207</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>29</v>
@@ -4198,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>28</v>
@@ -4212,16 +4495,19 @@
       <c r="M74" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N74" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>215</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>29</v>
@@ -4239,7 +4525,7 @@
         <v>2</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>28</v>
@@ -4253,16 +4539,22 @@
       <c r="M75" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O75" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>217</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>29</v>
@@ -4280,7 +4572,7 @@
         <v>2</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>28</v>
@@ -4293,6 +4585,12 @@
       </c>
       <c r="M76" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -4300,10 +4598,10 @@
         <v>219</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>29</v>
@@ -4321,7 +4619,7 @@
         <v>2</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>28</v>
@@ -4334,6 +4632,9 @@
       </c>
       <c r="M77" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
@@ -4341,10 +4642,10 @@
         <v>222</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>29</v>
@@ -4362,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>28</v>
@@ -4376,16 +4677,19 @@
       <c r="M78" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N78" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>232</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>29</v>
@@ -4403,13 +4707,13 @@
         <v>2</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>29</v>
@@ -4417,8 +4721,11 @@
       <c r="M79" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N79" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O79" s="3" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
@@ -4426,10 +4733,10 @@
         <v>238</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>29</v>
@@ -4447,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>28</v>
@@ -4460,6 +4767,9 @@
       </c>
       <c r="M80" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
@@ -4467,10 +4777,10 @@
         <v>239</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>29</v>
@@ -4488,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>28</v>
@@ -4501,6 +4811,9 @@
       </c>
       <c r="M81" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
@@ -4508,10 +4821,10 @@
         <v>248</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>29</v>
@@ -4529,7 +4842,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>28</v>
@@ -4542,6 +4855,9 @@
       </c>
       <c r="M82" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
@@ -4549,10 +4865,10 @@
         <v>254</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>29</v>
@@ -4570,7 +4886,7 @@
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>28</v>
@@ -4583,6 +4899,9 @@
       </c>
       <c r="M83" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
@@ -4590,10 +4909,10 @@
         <v>255</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>29</v>
@@ -4611,7 +4930,7 @@
         <v>2</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>28</v>
@@ -4624,6 +4943,9 @@
       </c>
       <c r="M84" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
@@ -4631,10 +4953,10 @@
         <v>257</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>29</v>
@@ -4652,7 +4974,7 @@
         <v>2</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>28</v>
@@ -4665,6 +4987,9 @@
       </c>
       <c r="M85" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
@@ -4672,10 +4997,10 @@
         <v>259</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>29</v>
@@ -4693,7 +5018,7 @@
         <v>2</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>28</v>
@@ -4706,6 +5031,9 @@
       </c>
       <c r="M86" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N86" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
@@ -4713,10 +5041,10 @@
         <v>346</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>29</v>
@@ -4734,7 +5062,7 @@
         <v>3</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>28</v>
@@ -4748,8 +5076,11 @@
       <c r="M87" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N87" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O87" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -4757,10 +5088,10 @@
         <v>358</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>29</v>
@@ -4778,7 +5109,7 @@
         <v>3</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>28</v>
@@ -4792,8 +5123,11 @@
       <c r="M88" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N88" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O88" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
@@ -4801,10 +5135,10 @@
         <v>359</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>29</v>
@@ -4822,7 +5156,7 @@
         <v>3</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>28</v>
@@ -4835,6 +5169,9 @@
       </c>
       <c r="M89" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
@@ -4842,10 +5179,10 @@
         <v>366</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>29</v>
@@ -4863,7 +5200,7 @@
         <v>3</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>28</v>
@@ -4876,6 +5213,9 @@
       </c>
       <c r="M90" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
@@ -4883,10 +5223,10 @@
         <v>369</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>29</v>
@@ -4904,7 +5244,7 @@
         <v>3</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>28</v>
@@ -4917,6 +5257,9 @@
       </c>
       <c r="M91" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
@@ -4924,10 +5267,10 @@
         <v>371</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>29</v>
@@ -4945,7 +5288,7 @@
         <v>3</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>28</v>
@@ -4958,6 +5301,9 @@
       </c>
       <c r="M92" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
@@ -4965,10 +5311,10 @@
         <v>372</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>29</v>
@@ -4986,7 +5332,7 @@
         <v>3</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>28</v>
@@ -5000,16 +5346,19 @@
       <c r="M93" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N93" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>373</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>29</v>
@@ -5027,7 +5376,7 @@
         <v>3</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>28</v>
@@ -5040,6 +5389,12 @@
       </c>
       <c r="M94" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O94" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -5047,10 +5402,10 @@
         <v>375</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>29</v>
@@ -5068,7 +5423,7 @@
         <v>3</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>28</v>
@@ -5082,8 +5437,11 @@
       <c r="M95" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N95" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O95" s="3" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
@@ -5091,10 +5449,10 @@
         <v>377</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>29</v>
@@ -5112,7 +5470,7 @@
         <v>3</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>28</v>
@@ -5126,8 +5484,11 @@
       <c r="M96" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N96" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O96" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
@@ -5135,10 +5496,10 @@
         <v>378</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>29</v>
@@ -5156,7 +5517,7 @@
         <v>3</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>28</v>
@@ -5169,6 +5530,9 @@
       </c>
       <c r="M97" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
@@ -5176,10 +5540,10 @@
         <v>386</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>29</v>
@@ -5197,7 +5561,7 @@
         <v>3</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>28</v>
@@ -5210,6 +5574,9 @@
       </c>
       <c r="M98" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
@@ -5217,10 +5584,10 @@
         <v>391</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>29</v>
@@ -5238,7 +5605,7 @@
         <v>3</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>28</v>
@@ -5251,6 +5618,9 @@
       </c>
       <c r="M99" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
@@ -5258,10 +5628,10 @@
         <v>394</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>29</v>
@@ -5279,7 +5649,7 @@
         <v>3</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>28</v>
@@ -5293,8 +5663,11 @@
       <c r="M100" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N100" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O100" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
@@ -5302,10 +5675,10 @@
         <v>395</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>29</v>
@@ -5323,7 +5696,7 @@
         <v>3</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J101" s="1" t="s">
         <v>28</v>
@@ -5336,6 +5709,9 @@
       </c>
       <c r="M101" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
@@ -5343,10 +5719,10 @@
         <v>69</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>29</v>
@@ -5377,6 +5753,9 @@
       </c>
       <c r="M102" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
@@ -5384,10 +5763,10 @@
         <v>70</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>29</v>
@@ -5418,6 +5797,9 @@
       </c>
       <c r="M103" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -5425,10 +5807,10 @@
         <v>71</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>29</v>
@@ -5460,8 +5842,11 @@
       <c r="M104" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N104" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O104" s="3" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
@@ -5469,10 +5854,10 @@
         <v>72</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>29</v>
@@ -5503,6 +5888,9 @@
       </c>
       <c r="M105" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
@@ -5510,10 +5898,10 @@
         <v>73</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>29</v>
@@ -5545,16 +5933,19 @@
       <c r="M106" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N106" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>74</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>29</v>
@@ -5585,6 +5976,12 @@
       </c>
       <c r="M107" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N107" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O107" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -5592,10 +5989,10 @@
         <v>75</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>29</v>
@@ -5627,8 +6024,11 @@
       <c r="M108" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N108" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O108" s="3" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
@@ -5636,10 +6036,10 @@
         <v>76</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>29</v>
@@ -5671,16 +6071,19 @@
       <c r="M109" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N109" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>77</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>29</v>
@@ -5712,19 +6115,22 @@
       <c r="M110" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N110" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O110" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>78</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>29</v>
@@ -5756,8 +6162,11 @@
       <c r="M111" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N111" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O111" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
@@ -5765,10 +6174,10 @@
         <v>79</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>29</v>
@@ -5799,6 +6208,9 @@
       </c>
       <c r="M112" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
@@ -5806,10 +6218,10 @@
         <v>80</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>29</v>
@@ -5840,6 +6252,12 @@
       </c>
       <c r="M113" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N113" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O113" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
@@ -5847,10 +6265,10 @@
         <v>81</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>29</v>
@@ -5881,6 +6299,9 @@
       </c>
       <c r="M114" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N114" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -5888,10 +6309,10 @@
         <v>82</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>29</v>
@@ -5923,8 +6344,11 @@
       <c r="M115" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N115" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O115" s="3" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.3">
@@ -5932,10 +6356,10 @@
         <v>83</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>29</v>
@@ -5966,6 +6390,9 @@
       </c>
       <c r="M116" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N116" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
@@ -5973,10 +6400,10 @@
         <v>209</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>29</v>
@@ -5994,7 +6421,7 @@
         <v>2</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J117" s="1" t="s">
         <v>28</v>
@@ -6007,6 +6434,9 @@
       </c>
       <c r="M117" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6014,10 +6444,10 @@
         <v>214</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>29</v>
@@ -6035,7 +6465,7 @@
         <v>2</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>28</v>
@@ -6049,8 +6479,11 @@
       <c r="M118" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N118" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O118" s="3" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.3">
@@ -6058,10 +6491,10 @@
         <v>216</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>29</v>
@@ -6079,7 +6512,7 @@
         <v>2</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J119" s="1" t="s">
         <v>28</v>
@@ -6092,6 +6525,9 @@
       </c>
       <c r="M119" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.3">
@@ -6099,10 +6535,10 @@
         <v>221</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>29</v>
@@ -6120,7 +6556,7 @@
         <v>2</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>28</v>
@@ -6133,6 +6569,9 @@
       </c>
       <c r="M120" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6140,10 +6579,10 @@
         <v>224</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>29</v>
@@ -6161,7 +6600,7 @@
         <v>2</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>28</v>
@@ -6175,19 +6614,22 @@
       <c r="M121" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N121" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O121" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>235</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>29</v>
@@ -6205,7 +6647,7 @@
         <v>2</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J122" s="1" t="s">
         <v>28</v>
@@ -6219,19 +6661,22 @@
       <c r="M122" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N122" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O122" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>236</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>29</v>
@@ -6249,7 +6694,7 @@
         <v>2</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J123" s="1" t="s">
         <v>28</v>
@@ -6263,8 +6708,11 @@
       <c r="M123" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N123" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O123" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.3">
@@ -6272,10 +6720,10 @@
         <v>240</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>29</v>
@@ -6293,7 +6741,7 @@
         <v>2</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J124" s="1" t="s">
         <v>28</v>
@@ -6306,6 +6754,9 @@
       </c>
       <c r="M124" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N124" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.3">
@@ -6313,10 +6764,10 @@
         <v>242</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>29</v>
@@ -6334,7 +6785,7 @@
         <v>2</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>28</v>
@@ -6347,6 +6798,9 @@
       </c>
       <c r="M125" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N125" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6354,10 +6808,10 @@
         <v>245</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>29</v>
@@ -6375,7 +6829,7 @@
         <v>2</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J126" s="1" t="s">
         <v>28</v>
@@ -6389,19 +6843,22 @@
       <c r="M126" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N126" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O126" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>251</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>29</v>
@@ -6419,7 +6876,7 @@
         <v>2</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J127" s="1" t="s">
         <v>28</v>
@@ -6433,8 +6890,11 @@
       <c r="M127" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N127" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O127" s="3" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6442,10 +6902,10 @@
         <v>253</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>29</v>
@@ -6463,7 +6923,7 @@
         <v>2</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J128" s="1" t="s">
         <v>28</v>
@@ -6477,8 +6937,11 @@
       <c r="M128" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N128" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O128" s="3" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
@@ -6486,10 +6949,10 @@
         <v>260</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>29</v>
@@ -6507,7 +6970,7 @@
         <v>2</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J129" s="1" t="s">
         <v>28</v>
@@ -6520,6 +6983,9 @@
       </c>
       <c r="M129" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
@@ -6527,10 +6993,10 @@
         <v>262</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>29</v>
@@ -6548,7 +7014,7 @@
         <v>2</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>28</v>
@@ -6562,16 +7028,19 @@
       <c r="M130" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N130" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>266</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>29</v>
@@ -6589,7 +7058,7 @@
         <v>2</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>28</v>
@@ -6602,6 +7071,12 @@
       </c>
       <c r="M131" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N131" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O131" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
@@ -6609,10 +7084,10 @@
         <v>338</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>29</v>
@@ -6630,7 +7105,7 @@
         <v>3</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J132" s="1" t="s">
         <v>28</v>
@@ -6643,6 +7118,9 @@
       </c>
       <c r="M132" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N132" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6650,10 +7128,10 @@
         <v>340</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>29</v>
@@ -6671,7 +7149,7 @@
         <v>3</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>28</v>
@@ -6685,19 +7163,22 @@
       <c r="M133" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N133" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O133" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>341</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>29</v>
@@ -6715,7 +7196,7 @@
         <v>3</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>28</v>
@@ -6729,8 +7210,11 @@
       <c r="M134" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N134" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O134" s="3" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
@@ -6738,10 +7222,10 @@
         <v>349</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>29</v>
@@ -6759,7 +7243,7 @@
         <v>3</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J135" s="1" t="s">
         <v>28</v>
@@ -6772,6 +7256,9 @@
       </c>
       <c r="M135" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
@@ -6779,10 +7266,10 @@
         <v>353</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>29</v>
@@ -6800,7 +7287,7 @@
         <v>3</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>28</v>
@@ -6813,6 +7300,9 @@
       </c>
       <c r="M136" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -6820,10 +7310,10 @@
         <v>354</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>29</v>
@@ -6841,7 +7331,7 @@
         <v>3</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>28</v>
@@ -6855,19 +7345,22 @@
       <c r="M137" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N137" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O137" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="138" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>355</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>29</v>
@@ -6885,7 +7378,7 @@
         <v>3</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J138" s="1" t="s">
         <v>28</v>
@@ -6899,8 +7392,11 @@
       <c r="M138" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N138" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="O138" s="3" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
@@ -6908,10 +7404,10 @@
         <v>357</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>29</v>
@@ -6929,7 +7425,7 @@
         <v>3</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J139" s="1" t="s">
         <v>28</v>
@@ -6942,6 +7438,9 @@
       </c>
       <c r="M139" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.3">
@@ -6949,10 +7448,10 @@
         <v>362</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>29</v>
@@ -6970,7 +7469,7 @@
         <v>3</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J140" s="1" t="s">
         <v>28</v>
@@ -6983,6 +7482,9 @@
       </c>
       <c r="M140" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.3">
@@ -6990,10 +7492,10 @@
         <v>365</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>29</v>
@@ -7011,7 +7513,7 @@
         <v>3</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J141" s="1" t="s">
         <v>28</v>
@@ -7024,6 +7526,9 @@
       </c>
       <c r="M141" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -7031,10 +7536,10 @@
         <v>367</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>29</v>
@@ -7052,7 +7557,7 @@
         <v>3</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>28</v>
@@ -7066,8 +7571,11 @@
       <c r="M142" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N142" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O142" s="3" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.3">
@@ -7075,10 +7583,10 @@
         <v>381</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>29</v>
@@ -7096,7 +7604,7 @@
         <v>3</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J143" s="1" t="s">
         <v>28</v>
@@ -7110,16 +7618,19 @@
       <c r="M143" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N143" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>383</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>29</v>
@@ -7137,7 +7648,7 @@
         <v>3</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J144" s="1" t="s">
         <v>28</v>
@@ -7150,6 +7661,12 @@
       </c>
       <c r="M144" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O144" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.3">
@@ -7157,10 +7674,10 @@
         <v>384</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>29</v>
@@ -7178,7 +7695,7 @@
         <v>3</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J145" s="1" t="s">
         <v>28</v>
@@ -7192,16 +7709,19 @@
       <c r="M145" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N145" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>385</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>29</v>
@@ -7219,7 +7739,7 @@
         <v>3</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J146" s="1" t="s">
         <v>28</v>
@@ -7233,8 +7753,11 @@
       <c r="M146" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N146" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O146" s="3" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added coral tag ID metadata which tracks the change of the tag number of the colony by the field tag
</commit_message>
<xml_diff>
--- a/metadata/E5_2020_Timeseries_Sample_Metadata_Sheet.xlsx
+++ b/metadata/E5_2020_Timeseries_Sample_Metadata_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcone\Documents\URI\Lab-Notebook\urol-e5\timeseries\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71102F65-4B55-4BF6-B4A5-BCE978D4C55B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0097DE7F-8DBE-4096-AEB1-90EF685818B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2952" windowWidth="17280" windowHeight="9408" xr2:uid="{A9225978-0C17-4C60-8E40-23766E55B839}"/>
   </bookViews>
@@ -1091,9 +1091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2420B75-8665-4DB7-A7B4-8B4461FB7AD9}">
   <dimension ref="A1:O146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O55" sqref="O55"/>
+      <selection pane="topRight" activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>